<commit_message>
Live Trading Trend Done
</commit_message>
<xml_diff>
--- a/data/Forex Total Result no ema update.xlsx
+++ b/data/Forex Total Result no ema update.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Techincal Analysis Program\MT5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Techincal Analysis Program\MT5\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55B7085-64AB-4C86-A78E-C8E069295530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90A06A1-A1AA-4841-9BA9-C337FC5B46BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,7 +684,7 @@
     <col min="2" max="2" width="26.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.88671875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="7" max="7" width="16" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -703,7 +703,7 @@
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -741,7 +741,7 @@
       <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H2">
@@ -779,7 +779,7 @@
       <c r="F3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H3">
@@ -817,7 +817,7 @@
       <c r="F4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H4">
@@ -855,7 +855,7 @@
       <c r="F5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H5">
@@ -893,7 +893,7 @@
       <c r="F6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H6">
@@ -931,7 +931,7 @@
       <c r="F7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H7">
@@ -969,7 +969,7 @@
       <c r="F8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="3" t="s">
         <v>35</v>
       </c>
       <c r="H8">
@@ -1007,7 +1007,7 @@
       <c r="F9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H9">
@@ -1045,7 +1045,7 @@
       <c r="F10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="H10">
@@ -1083,7 +1083,7 @@
       <c r="F11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="3" t="s">
         <v>44</v>
       </c>
       <c r="H11">
@@ -1121,7 +1121,7 @@
       <c r="F12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="3" t="s">
         <v>47</v>
       </c>
       <c r="H12">
@@ -1159,7 +1159,7 @@
       <c r="F13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="3" t="s">
         <v>50</v>
       </c>
       <c r="H13">
@@ -1197,7 +1197,7 @@
       <c r="F14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="3" t="s">
         <v>53</v>
       </c>
       <c r="H14">
@@ -1235,7 +1235,7 @@
       <c r="F15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="3" t="s">
         <v>56</v>
       </c>
       <c r="H15">
@@ -1273,7 +1273,7 @@
       <c r="F16" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="3" t="s">
         <v>59</v>
       </c>
       <c r="H16">
@@ -1311,7 +1311,7 @@
       <c r="F17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="3" t="s">
         <v>63</v>
       </c>
       <c r="H17">
@@ -1349,7 +1349,7 @@
       <c r="F18" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="3" t="s">
         <v>66</v>
       </c>
       <c r="H18">
@@ -1387,7 +1387,7 @@
       <c r="F19" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="3" t="s">
         <v>69</v>
       </c>
       <c r="H19">
@@ -1425,7 +1425,7 @@
       <c r="F20" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="3" t="s">
         <v>72</v>
       </c>
       <c r="H20">
@@ -1463,7 +1463,7 @@
       <c r="F21" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="3" t="s">
         <v>75</v>
       </c>
       <c r="H21">
@@ -1501,7 +1501,7 @@
       <c r="F22" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="3" t="s">
         <v>78</v>
       </c>
       <c r="H22">
@@ -1539,7 +1539,7 @@
       <c r="F23" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="3" t="s">
         <v>82</v>
       </c>
       <c r="H23">
@@ -1577,7 +1577,7 @@
       <c r="F24" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="3" t="s">
         <v>85</v>
       </c>
       <c r="H24">

</xml_diff>